<commit_message>
Final version of the BPS sample data files
</commit_message>
<xml_diff>
--- a/seed/tests/data/building-performance-standards-sample-2023.xlsx
+++ b/seed/tests/data/building-performance-standards-sample-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77848B8-AD00-6E49-A312-8589251EB456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2EC9E-77D1-9248-B77A-51A8E74BCB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1420" windowWidth="38400" windowHeight="19840" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="40020" yWindow="3580" windowWidth="21600" windowHeight="19840" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Property Name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Weather Normalized Site EUI</t>
   </si>
   <si>
-    <t>Medstar POB North Tower</t>
-  </si>
-  <si>
     <t>106 IRVING ST NW</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>admin@companya.com</t>
   </si>
   <si>
-    <t>1801 Pennsylvania Ave.</t>
-  </si>
-  <si>
     <t>Office</t>
   </si>
   <si>
@@ -127,12 +121,6 @@
     <t>GSA: 300 E Street SW</t>
   </si>
   <si>
-    <t>0300 E ST SW</t>
-  </si>
-  <si>
-    <t>WELLS REIT/INDEPENDENCE SQUARE LLC</t>
-  </si>
-  <si>
     <t>admin@companyc.com</t>
   </si>
   <si>
@@ -148,18 +136,9 @@
     <t>admin@companyd.com</t>
   </si>
   <si>
-    <t>President Madison Apartments</t>
-  </si>
-  <si>
     <t>Multifamily</t>
   </si>
   <si>
-    <t>1908 FLORIDA AV NW</t>
-  </si>
-  <si>
-    <t>BDC PRESIDENT MADISON LLC</t>
-  </si>
-  <si>
     <t>admin@companye.com</t>
   </si>
   <si>
@@ -178,9 +157,6 @@
     <t>15th and H Street Associates LLP</t>
   </si>
   <si>
-    <t>733 15TH ST NW</t>
-  </si>
-  <si>
     <t>15TH AND H STREET ASSOCIATES LP</t>
   </si>
   <si>
@@ -202,19 +178,46 @@
     <t>admin@companyh.com</t>
   </si>
   <si>
-    <t>DPW Vehicle Maintenance Facility 2</t>
-  </si>
-  <si>
-    <t>Service-Repair</t>
-  </si>
-  <si>
-    <t>1242 MOUNT OLIVET RD NE</t>
-  </si>
-  <si>
-    <t>GOVERNMENT OF THE DISTRICT OF COLUMBIA DEPARTMENT OF GENERAL SERVICES</t>
-  </si>
-  <si>
     <t>admin@companyi.com</t>
+  </si>
+  <si>
+    <t>Medstar POB South Tower</t>
+  </si>
+  <si>
+    <t>1801 Pennsylvania Avenue, LLC</t>
+  </si>
+  <si>
+    <t>300 E ST SW</t>
+  </si>
+  <si>
+    <t>TWO INDEPENDENCE HANA OW LLC</t>
+  </si>
+  <si>
+    <t>Hampton House</t>
+  </si>
+  <si>
+    <t>2700 CONNECTICUT AVENUE NW</t>
+  </si>
+  <si>
+    <t>2700 CONECTICUT AVENUE LLC</t>
+  </si>
+  <si>
+    <t>1428 H ST NW</t>
+  </si>
+  <si>
+    <t>School Without Walls @ Francis Stevens</t>
+  </si>
+  <si>
+    <t>K-12 School</t>
+  </si>
+  <si>
+    <t>2425 N STREET NW</t>
+  </si>
+  <si>
+    <t>GHGI Target</t>
+  </si>
+  <si>
+    <t>GHGI Target Year</t>
   </si>
 </sst>
 </file>
@@ -244,6 +247,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -257,14 +266,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -274,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -282,21 +283,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4367F287-F053-B14B-BB78-7F2A1A8270CC}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{FC32E4A8-5101-754C-BA01-BA4BA25B0A66}"/>
@@ -611,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AAF8DA-FAFC-5247-8BBA-26096DB3751B}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,133 +638,133 @@
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11911</v>
       </c>
       <c r="B2">
-        <v>21537666</v>
+        <v>22178843</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
       <c r="H2">
         <v>20010</v>
       </c>
       <c r="I2">
-        <v>1967</v>
-      </c>
-      <c r="J2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="L2">
-        <v>106517</v>
-      </c>
-      <c r="M2">
-        <v>6.7</v>
-      </c>
-      <c r="N2">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="O2" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P2">
-        <v>88</v>
+        <v>76319</v>
+      </c>
+      <c r="O2" s="2">
+        <v>45291</v>
       </c>
       <c r="Q2">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S2">
+        <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12227</v>
       </c>
       <c r="B3">
-        <v>21537667</v>
+        <v>22178844</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
       <c r="H3">
         <v>20006</v>
@@ -756,52 +772,46 @@
       <c r="I3">
         <v>1991</v>
       </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>28</v>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
       </c>
       <c r="L3">
-        <v>220131</v>
-      </c>
-      <c r="M3">
-        <v>7.6</v>
-      </c>
-      <c r="N3">
-        <v>70.599999999999994</v>
-      </c>
-      <c r="O3" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P3">
-        <v>138</v>
+        <v>227440.2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>45291</v>
       </c>
       <c r="Q3">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S3">
+        <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>17971</v>
       </c>
       <c r="B4">
-        <v>21537668</v>
+        <v>22178845</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
       </c>
       <c r="H4">
         <v>20546</v>
@@ -809,52 +819,46 @@
       <c r="I4">
         <v>1991</v>
       </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>32</v>
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
       </c>
       <c r="L4">
-        <v>659773</v>
-      </c>
-      <c r="M4">
-        <v>6.4</v>
-      </c>
-      <c r="N4">
-        <v>59.6</v>
-      </c>
-      <c r="O4" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P4">
-        <v>138</v>
+        <v>627655</v>
+      </c>
+      <c r="O4" s="2">
+        <v>45291</v>
       </c>
       <c r="Q4">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S4">
+        <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>21381</v>
       </c>
       <c r="B5">
-        <v>21537669</v>
+        <v>22178846</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
       </c>
       <c r="H5">
         <v>20036</v>
@@ -862,158 +866,140 @@
       <c r="I5">
         <v>1962</v>
       </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>36</v>
+      <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
       </c>
       <c r="L5">
-        <v>65273</v>
-      </c>
-      <c r="M5">
-        <v>7.2</v>
-      </c>
-      <c r="N5">
-        <v>82.1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P5">
-        <v>138</v>
+        <v>58717</v>
+      </c>
+      <c r="O5" s="2">
+        <v>45291</v>
       </c>
       <c r="Q5">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S5">
+        <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>21404</v>
       </c>
       <c r="B6">
-        <v>21537670</v>
+        <v>22482006</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
       <c r="H6">
-        <v>20009</v>
+        <v>20008</v>
       </c>
       <c r="I6">
-        <v>1908</v>
-      </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>41</v>
+        <v>1921</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
       </c>
       <c r="L6">
-        <v>86166</v>
-      </c>
-      <c r="M6">
-        <v>3.9</v>
-      </c>
-      <c r="N6">
-        <v>61.1</v>
-      </c>
-      <c r="O6" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P6">
-        <v>62</v>
+        <v>83580</v>
+      </c>
+      <c r="O6" s="2">
+        <v>45291</v>
       </c>
       <c r="Q6">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S6">
+        <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>21405</v>
       </c>
       <c r="B7">
-        <v>21537671</v>
+        <v>22178848</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
       <c r="H7">
-        <v>20007</v>
+        <v>20005</v>
       </c>
       <c r="I7">
         <v>2004</v>
       </c>
-      <c r="J7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>45</v>
+      <c r="J7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
       </c>
       <c r="L7">
-        <v>134036</v>
-      </c>
-      <c r="M7">
-        <v>7.2</v>
-      </c>
-      <c r="N7">
-        <v>88.8</v>
-      </c>
-      <c r="O7" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P7">
-        <v>62</v>
+        <v>145697</v>
+      </c>
+      <c r="O7" s="2">
+        <v>45291</v>
       </c>
       <c r="Q7">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S7">
+        <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21368</v>
       </c>
       <c r="B8">
-        <v>21537672</v>
+        <v>22178849</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
       </c>
       <c r="H8">
         <v>20005</v>
@@ -1021,52 +1007,46 @@
       <c r="I8">
         <v>1912</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>49</v>
+      <c r="J8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
       </c>
       <c r="L8">
         <v>230129</v>
       </c>
-      <c r="M8">
-        <v>3.7</v>
-      </c>
-      <c r="N8">
-        <v>44.1</v>
-      </c>
-      <c r="O8" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P8">
-        <v>62</v>
+      <c r="O8" s="2">
+        <v>45291</v>
       </c>
       <c r="Q8">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S8">
+        <v>2024</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>21378</v>
       </c>
       <c r="B9">
-        <v>21537673</v>
+        <v>22178850</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
         <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
       </c>
       <c r="H9">
         <v>20003</v>
@@ -1074,94 +1054,75 @@
       <c r="I9">
         <v>1880</v>
       </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>54</v>
+      <c r="J9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
       </c>
       <c r="L9">
         <v>29906</v>
       </c>
-      <c r="M9">
-        <v>9.1</v>
-      </c>
-      <c r="N9">
-        <v>113.1</v>
-      </c>
-      <c r="O9" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P9">
-        <v>113</v>
+      <c r="O9" s="2">
+        <v>45291</v>
       </c>
       <c r="Q9">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S9">
+        <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21426</v>
       </c>
       <c r="B10">
-        <v>21537674</v>
+        <v>22482007</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
       <c r="H10">
-        <v>20002</v>
-      </c>
-      <c r="J10" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>59</v>
+        <v>20037</v>
+      </c>
+      <c r="I10">
+        <v>1924</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>47</v>
       </c>
       <c r="L10">
-        <v>134114</v>
-      </c>
-      <c r="M10">
-        <v>9.5</v>
-      </c>
-      <c r="N10">
-        <v>146.19999999999999</v>
-      </c>
-      <c r="O10" s="1">
-        <v>43100</v>
-      </c>
-      <c r="P10">
-        <v>152</v>
+        <v>127991</v>
+      </c>
+      <c r="O10" s="2">
+        <v>45291</v>
       </c>
       <c r="Q10">
-        <v>2018</v>
+        <v>2024</v>
+      </c>
+      <c r="S10">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" display="mailto:admin@companya.com" xr:uid="{5D9E569B-C2E8-664B-947D-065906FF283E}"/>
-    <hyperlink ref="K3" r:id="rId2" display="mailto:admin@companyb.com" xr:uid="{47AB2A2A-A505-C247-B1DD-53A7FC6515EE}"/>
-    <hyperlink ref="K4" r:id="rId3" display="mailto:admin@companyc.com" xr:uid="{91D17F89-FCBD-3F43-A522-B4B547E4D180}"/>
-    <hyperlink ref="K5" r:id="rId4" display="mailto:admin@companyd.com" xr:uid="{FECC3924-08BC-9244-BCC1-B1E30403F411}"/>
-    <hyperlink ref="K6" r:id="rId5" display="mailto:admin@companye.com" xr:uid="{9FF81FBC-30D4-1544-8B3B-CE7BC20C47A9}"/>
-    <hyperlink ref="K7" r:id="rId6" display="mailto:admin@companyf.com" xr:uid="{FDDE0CFB-B11A-A941-A49A-6A3A1F02849B}"/>
-    <hyperlink ref="K8" r:id="rId7" display="mailto:admin@companyg.com" xr:uid="{A1DD5738-6AAF-6941-9602-A938A28AC10A}"/>
-    <hyperlink ref="K9" r:id="rId8" display="mailto:admin@companyh.com" xr:uid="{0338C2A9-86B3-1341-B154-5928856931EE}"/>
-    <hyperlink ref="K10" r:id="rId9" display="mailto:admin@companyi.com" xr:uid="{261BF134-279F-354B-9792-477E6A92F3E3}"/>
-  </hyperlinks>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>